<commit_message>
updated main effects file of lmb
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/habitat-season/lmb/glmm_main_effects_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/habitat-season/lmb/glmm_main_effects_hab_season_lmb.xlsx
@@ -1,46 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\accel-glmm-results\habitat-season\lmb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158C1926-ED9F-4742-A810-47ABDAFB3E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">season</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_type:season</t>
+    <t>term</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>p.value</t>
+  </si>
+  <si>
+    <t>habitat_type</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>habitat_type:season</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -76,6 +83,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,14 +373,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,50 +396,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>85.5428312652268</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>85.542831265226795</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.0000000000000000116359219675931</v>
+      <c r="D2">
+        <v>1.1635921967593099E-17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>3267.31855575395</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>159.77401225967</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.0000000000000000000000000000360763509549953</v>
+      <c r="D4">
+        <v>3.6076350954995301E-29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>